<commit_message>
Implement Helpers and Modify DB(xlsx) as Data Structure Changed
</commit_message>
<xml_diff>
--- a/absolutely_essential_words_504.xlsx
+++ b/absolutely_essential_words_504.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/dev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macuser/Desktop/portfolio/wordama/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27082D08-9DFE-7848-96A3-49EC0F01C651}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lesson1-6" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>word</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,24 +68,27 @@
   <si>
     <t>ability to say the right thing</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrong_nums</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -114,13 +118,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -388,53 +395,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>